<commit_message>
Updates to website and UTF characters update in profile script
Added Lisa profile picture, updated Danielle and Eriks text for consistency and correct some errors.

Also updated profile creation script to deal with weird characters.
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Danielle_Greco/Author_form_DanielleGreco.xlsx
+++ b/website_content_creation/authors/Danielle_Greco/Author_form_DanielleGreco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Danielle_Greco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{D30DED2D-0B73-4A8C-BEF5-76B71931AC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32D2DF38-2002-4D1B-9E28-A2F453FC5378}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{D30DED2D-0B73-4A8C-BEF5-76B71931AC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209AF736-9549-49A9-9778-232A4995D351}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="1845" windowWidth="28770" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,13 +147,13 @@
     <t>https://twitter.com/dan13llegreco</t>
   </si>
   <si>
-    <t>Great Lakes Forestry Centre</t>
-  </si>
-  <si>
     <t>https://www.nrcan.gc.ca/science-and-data/research-centres-and-labs/forestry-research-centres/great-lakes-forestry-centre/13459</t>
   </si>
   <si>
     <t>Watershed Ecology Team</t>
+  </si>
+  <si>
+    <t>Great Lakes Forestry Centre, Natural Resources Canada</t>
   </si>
 </sst>
 </file>
@@ -572,6 +572,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,7 +582,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -913,8 +913,8 @@
       <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>42</v>
+      <c r="B14" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -926,11 +926,11 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
@@ -982,10 +982,10 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="37"/>
+      <c r="B24" s="38"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -997,10 +997,10 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="32" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>